<commit_message>
Small changes before start
- small corrections between excel and code
</commit_message>
<xml_diff>
--- a/bin/Equipment Traceability.xlsx
+++ b/bin/Equipment Traceability.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\Eyonai\Documents\GitHub\Baseline-Check\bin\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B49D2268-4624-44D5-84F5-6AA00A8AFE25}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{805FA223-FAB9-4905-8784-7FD90D26D007}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="30612" yWindow="-108" windowWidth="30936" windowHeight="17040" activeTab="10" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-135" yWindow="-135" windowWidth="51870" windowHeight="21360" activeTab="1" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="System" sheetId="1" r:id="rId1"/>
@@ -35,7 +35,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1226" uniqueCount="655">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="1233" uniqueCount="658">
   <si>
     <t>Patch Unit</t>
   </si>
@@ -2029,6 +2029,15 @@
   </si>
   <si>
     <t>Recording System</t>
+  </si>
+  <si>
+    <t>CP-4458-07F_CFI 9</t>
+  </si>
+  <si>
+    <t>Pacer Type</t>
+  </si>
+  <si>
+    <t>Pacer Serial Number</t>
   </si>
 </sst>
 </file>
@@ -2895,6 +2904,9 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
       <alignment horizontal="left"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment wrapText="1"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -2904,12 +2916,12 @@
     <xf numFmtId="0" fontId="16" fillId="17" borderId="0" xfId="2" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top"/>
     </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
     <xf numFmtId="0" fontId="5" fillId="6" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
@@ -2925,120 +2937,120 @@
     <xf numFmtId="0" fontId="5" fillId="0" borderId="19" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="top" wrapText="1"/>
     </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="8" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="9" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center" vertical="center"/>
     </xf>
     <xf numFmtId="0" fontId="9" fillId="11" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="11" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="12" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
     <xf numFmtId="0" fontId="9" fillId="12" borderId="13" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="12" borderId="30" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="18" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="20" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="3" borderId="14" xfId="0" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="12" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="25" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="26" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="8" fillId="9" borderId="27" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="31" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="8" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="10" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center" wrapText="1"/>
-    </xf>
-    <xf numFmtId="0" fontId="9" fillId="11" borderId="29" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center" vertical="center"/>
-    </xf>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="17" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
     </xf>
@@ -3050,9 +3062,6 @@
     </xf>
     <xf numFmtId="0" fontId="4" fillId="5" borderId="32" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center"/>
-    </xf>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
-      <alignment wrapText="1"/>
     </xf>
   </cellXfs>
   <cellStyles count="3">
@@ -3404,7 +3413,7 @@
   <dimension ref="A1:Q65"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection activeCell="G9" sqref="G9"/>
+      <selection activeCell="F4" sqref="F4"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="8.69921875" defaultRowHeight="13.8"/>
@@ -3423,18 +3432,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="86" t="s">
+      <c r="A1" s="87" t="s">
         <v>56</v>
       </c>
-      <c r="B1" s="86"/>
-      <c r="C1" s="86"/>
-      <c r="D1" s="86"/>
-      <c r="E1" s="86"/>
-      <c r="F1" s="86"/>
-      <c r="G1" s="86"/>
-      <c r="H1" s="86"/>
-      <c r="I1" s="86"/>
-      <c r="J1" s="86"/>
+      <c r="B1" s="87"/>
+      <c r="C1" s="87"/>
+      <c r="D1" s="87"/>
+      <c r="E1" s="87"/>
+      <c r="F1" s="87"/>
+      <c r="G1" s="87"/>
+      <c r="H1" s="87"/>
+      <c r="I1" s="87"/>
+      <c r="J1" s="87"/>
     </row>
     <row r="2" spans="1:11" ht="15.6">
       <c r="A2" s="44" t="s">
@@ -4257,12 +4266,12 @@
       <c r="F41" s="66"/>
       <c r="G41" s="66"/>
       <c r="H41" s="66"/>
-      <c r="M41" s="87" t="s">
+      <c r="M41" s="88" t="s">
         <v>584</v>
       </c>
-      <c r="N41" s="88"/>
-      <c r="O41" s="88"/>
-      <c r="P41" s="88"/>
+      <c r="N41" s="89"/>
+      <c r="O41" s="89"/>
+      <c r="P41" s="89"/>
     </row>
     <row r="42" spans="1:17" ht="14.4">
       <c r="A42" s="66"/>
@@ -4523,25 +4532,25 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:17">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="100" t="s">
         <v>174</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
-      <c r="J1" s="96"/>
-      <c r="K1" s="96"/>
-      <c r="L1" s="96"/>
-      <c r="M1" s="96"/>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
-      <c r="Q1" s="96"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
+      <c r="J1" s="100"/>
+      <c r="K1" s="100"/>
+      <c r="L1" s="100"/>
+      <c r="M1" s="100"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
+      <c r="Q1" s="100"/>
     </row>
     <row r="2" spans="1:17" ht="15.6">
       <c r="A2" s="40" t="s">
@@ -4813,7 +4822,7 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{862B71AC-4844-4212-8571-242447F6BD8F}">
   <dimension ref="A1:I3"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
+    <sheetView workbookViewId="0">
       <selection activeCell="L17" activeCellId="1" sqref="F8 L17"/>
     </sheetView>
   </sheetViews>
@@ -4825,18 +4834,18 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:9">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="100" t="s">
         <v>127</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="F1" s="96" t="s">
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="F1" s="100" t="s">
         <v>521</v>
       </c>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
     </row>
     <row r="2" spans="1:9" ht="15.6">
       <c r="A2" s="40" t="s">
@@ -4903,8 +4912,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{8B33D2A6-4CFD-4DE8-AF6E-58921D3DF7AE}">
   <dimension ref="A1:AE107"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="S20" sqref="S20"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="I23" sqref="I23"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -4914,7 +4923,7 @@
     <col min="3" max="3" width="14.3984375" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.796875" bestFit="1" customWidth="1"/>
     <col min="5" max="5" width="16.09765625" bestFit="1" customWidth="1"/>
-    <col min="7" max="7" width="14.69921875" bestFit="1" customWidth="1"/>
+    <col min="7" max="7" width="21.69921875" bestFit="1" customWidth="1"/>
     <col min="8" max="8" width="12.69921875" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
@@ -6145,7 +6154,7 @@
         <v>218</v>
       </c>
       <c r="D41" s="65" t="s">
-        <v>32</v>
+        <v>655</v>
       </c>
       <c r="E41" s="65" t="s">
         <v>173</v>
@@ -6169,7 +6178,25 @@
       <c r="AD41" s="3"/>
       <c r="AE41" s="3"/>
     </row>
-    <row r="42" spans="1:31">
+    <row r="42" spans="1:31" ht="14.4">
+      <c r="A42" s="65" t="s">
+        <v>245</v>
+      </c>
+      <c r="B42" s="65" t="s">
+        <v>45</v>
+      </c>
+      <c r="C42" s="65" t="s">
+        <v>218</v>
+      </c>
+      <c r="D42" s="65" t="s">
+        <v>35</v>
+      </c>
+      <c r="G42" s="65" t="s">
+        <v>613</v>
+      </c>
+      <c r="H42" s="65" t="s">
+        <v>614</v>
+      </c>
       <c r="W42" s="15"/>
       <c r="X42" s="7"/>
       <c r="Y42" s="7"/>
@@ -6500,26 +6527,26 @@
       <c r="AE71" s="3"/>
     </row>
     <row r="72" spans="23:31">
-      <c r="W72" s="91"/>
-      <c r="X72" s="93"/>
-      <c r="Y72" s="93"/>
+      <c r="W72" s="92"/>
+      <c r="X72" s="94"/>
+      <c r="Y72" s="94"/>
       <c r="Z72" s="18"/>
-      <c r="AA72" s="93"/>
-      <c r="AB72" s="93"/>
-      <c r="AC72" s="95"/>
-      <c r="AD72" s="89"/>
-      <c r="AE72" s="89"/>
+      <c r="AA72" s="94"/>
+      <c r="AB72" s="94"/>
+      <c r="AC72" s="96"/>
+      <c r="AD72" s="91"/>
+      <c r="AE72" s="91"/>
     </row>
     <row r="73" spans="23:31">
-      <c r="W73" s="92"/>
-      <c r="X73" s="94"/>
-      <c r="Y73" s="94"/>
+      <c r="W73" s="93"/>
+      <c r="X73" s="95"/>
+      <c r="Y73" s="95"/>
       <c r="Z73" s="19"/>
-      <c r="AA73" s="94"/>
-      <c r="AB73" s="94"/>
-      <c r="AC73" s="95"/>
-      <c r="AD73" s="89"/>
-      <c r="AE73" s="89"/>
+      <c r="AA73" s="95"/>
+      <c r="AB73" s="95"/>
+      <c r="AC73" s="96"/>
+      <c r="AD73" s="91"/>
+      <c r="AE73" s="91"/>
     </row>
     <row r="74" spans="23:31">
       <c r="W74" s="15"/>
@@ -9048,21 +9075,21 @@
   </cols>
   <sheetData>
     <row r="1" spans="2:17" ht="15.6" customHeight="1" thickBot="1">
-      <c r="B1" s="121" t="s">
+      <c r="B1" s="97" t="s">
         <v>64</v>
       </c>
-      <c r="C1" s="122"/>
+      <c r="C1" s="98"/>
       <c r="D1" s="79"/>
-      <c r="G1" s="121"/>
-      <c r="H1" s="122"/>
-      <c r="J1" s="121"/>
-      <c r="K1" s="122"/>
-      <c r="M1" s="123" t="s">
+      <c r="G1" s="97"/>
+      <c r="H1" s="98"/>
+      <c r="J1" s="97"/>
+      <c r="K1" s="98"/>
+      <c r="M1" s="99" t="s">
         <v>86</v>
       </c>
-      <c r="N1" s="96"/>
-      <c r="O1" s="96"/>
-      <c r="P1" s="96"/>
+      <c r="N1" s="100"/>
+      <c r="O1" s="100"/>
+      <c r="P1" s="100"/>
     </row>
     <row r="2" spans="2:17" ht="15.6">
       <c r="B2" s="30" t="s">
@@ -9076,12 +9103,12 @@
       <c r="H2" s="33"/>
       <c r="J2" s="30"/>
       <c r="K2" s="33"/>
-      <c r="M2" s="127" t="s">
+      <c r="M2" s="104" t="s">
         <v>161</v>
       </c>
-      <c r="N2" s="128"/>
-      <c r="O2" s="128"/>
-      <c r="P2" s="129"/>
+      <c r="N2" s="105"/>
+      <c r="O2" s="105"/>
+      <c r="P2" s="106"/>
     </row>
     <row r="3" spans="2:17" ht="15.6">
       <c r="G3" s="34"/>
@@ -9128,43 +9155,43 @@
       <c r="D5" s="41"/>
       <c r="J5" s="36"/>
       <c r="K5" s="37"/>
-      <c r="M5" s="100" t="s">
+      <c r="M5" s="110" t="s">
         <v>11</v>
       </c>
-      <c r="N5" s="97" t="s">
+      <c r="N5" s="112" t="s">
         <v>347</v>
       </c>
-      <c r="O5" s="97" t="s">
+      <c r="O5" s="112" t="s">
         <v>163</v>
       </c>
-      <c r="P5" s="104" t="s">
+      <c r="P5" s="107" t="s">
         <v>458</v>
       </c>
     </row>
     <row r="6" spans="2:17" ht="14.4" customHeight="1" thickBot="1">
-      <c r="M6" s="101"/>
-      <c r="N6" s="98"/>
-      <c r="O6" s="98"/>
-      <c r="P6" s="105"/>
+      <c r="M6" s="116"/>
+      <c r="N6" s="118"/>
+      <c r="O6" s="118"/>
+      <c r="P6" s="108"/>
     </row>
     <row r="7" spans="2:17" ht="13.95" customHeight="1">
-      <c r="B7" s="121" t="s">
+      <c r="B7" s="97" t="s">
         <v>65</v>
       </c>
-      <c r="C7" s="122"/>
+      <c r="C7" s="98"/>
       <c r="D7" s="79"/>
-      <c r="G7" s="121" t="s">
+      <c r="G7" s="97" t="s">
         <v>76</v>
       </c>
-      <c r="H7" s="122"/>
-      <c r="J7" s="121" t="s">
+      <c r="H7" s="98"/>
+      <c r="J7" s="97" t="s">
         <v>79</v>
       </c>
-      <c r="K7" s="122"/>
-      <c r="M7" s="102"/>
-      <c r="N7" s="103"/>
-      <c r="O7" s="103"/>
-      <c r="P7" s="106"/>
+      <c r="K7" s="98"/>
+      <c r="M7" s="111"/>
+      <c r="N7" s="113"/>
+      <c r="O7" s="113"/>
+      <c r="P7" s="133"/>
     </row>
     <row r="8" spans="2:17" ht="46.8">
       <c r="B8" s="30" t="s">
@@ -9250,13 +9277,13 @@
       <c r="K10" s="35" t="s">
         <v>305</v>
       </c>
-      <c r="M10" s="100" t="s">
+      <c r="M10" s="110" t="s">
         <v>92</v>
       </c>
-      <c r="N10" s="97" t="s">
+      <c r="N10" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="O10" s="131" t="s">
+      <c r="O10" s="114" t="s">
         <v>165</v>
       </c>
       <c r="P10" s="70" t="s">
@@ -9277,9 +9304,9 @@
       <c r="K11" s="77" t="s">
         <v>447</v>
       </c>
-      <c r="M11" s="102"/>
-      <c r="N11" s="103"/>
-      <c r="O11" s="132"/>
+      <c r="M11" s="111"/>
+      <c r="N11" s="113"/>
+      <c r="O11" s="115"/>
       <c r="P11" s="32"/>
     </row>
     <row r="12" spans="2:17" ht="13.95" customHeight="1">
@@ -9294,16 +9321,16 @@
       <c r="K12" s="35" t="s">
         <v>304</v>
       </c>
-      <c r="M12" s="100" t="s">
+      <c r="M12" s="110" t="s">
         <v>93</v>
       </c>
-      <c r="N12" s="97" t="s">
+      <c r="N12" s="112" t="s">
         <v>91</v>
       </c>
-      <c r="O12" s="97" t="s">
+      <c r="O12" s="112" t="s">
         <v>166</v>
       </c>
-      <c r="P12" s="104" t="s">
+      <c r="P12" s="107" t="s">
         <v>356</v>
       </c>
       <c r="Q12" s="74" t="s">
@@ -9324,10 +9351,10 @@
       <c r="K13" s="35" t="s">
         <v>306</v>
       </c>
-      <c r="M13" s="101"/>
-      <c r="N13" s="98"/>
-      <c r="O13" s="98"/>
-      <c r="P13" s="105"/>
+      <c r="M13" s="116"/>
+      <c r="N13" s="118"/>
+      <c r="O13" s="118"/>
+      <c r="P13" s="108"/>
       <c r="Q13" s="75" t="s">
         <v>349</v>
       </c>
@@ -9345,10 +9372,10 @@
       <c r="K14" s="35" t="s">
         <v>362</v>
       </c>
-      <c r="M14" s="101"/>
-      <c r="N14" s="98"/>
-      <c r="O14" s="98"/>
-      <c r="P14" s="105"/>
+      <c r="M14" s="116"/>
+      <c r="N14" s="118"/>
+      <c r="O14" s="118"/>
+      <c r="P14" s="108"/>
       <c r="Q14" s="75" t="s">
         <v>350</v>
       </c>
@@ -9362,10 +9389,10 @@
       </c>
       <c r="J15" s="34"/>
       <c r="K15" s="35"/>
-      <c r="M15" s="133"/>
-      <c r="N15" s="99"/>
-      <c r="O15" s="99"/>
-      <c r="P15" s="130"/>
+      <c r="M15" s="117"/>
+      <c r="N15" s="119"/>
+      <c r="O15" s="119"/>
+      <c r="P15" s="109"/>
       <c r="Q15" s="75" t="s">
         <v>351</v>
       </c>
@@ -9375,18 +9402,18 @@
       <c r="K16" s="37"/>
     </row>
     <row r="17" spans="1:16" ht="16.2" thickBot="1">
-      <c r="M17" s="124" t="s">
+      <c r="M17" s="101" t="s">
         <v>160</v>
       </c>
-      <c r="N17" s="125"/>
-      <c r="O17" s="125"/>
-      <c r="P17" s="126"/>
+      <c r="N17" s="102"/>
+      <c r="O17" s="102"/>
+      <c r="P17" s="103"/>
     </row>
     <row r="18" spans="1:16" ht="15.6">
-      <c r="G18" s="121" t="s">
+      <c r="G18" s="97" t="s">
         <v>72</v>
       </c>
-      <c r="H18" s="122"/>
+      <c r="H18" s="98"/>
       <c r="M18" s="58" t="s">
         <v>28</v>
       </c>
@@ -9421,33 +9448,33 @@
       <c r="H20" s="37" t="s">
         <v>74</v>
       </c>
-      <c r="M20" s="107" t="s">
+      <c r="M20" s="123" t="s">
         <v>11</v>
       </c>
-      <c r="N20" s="110"/>
-      <c r="O20" s="110"/>
-      <c r="P20" s="113"/>
+      <c r="N20" s="125"/>
+      <c r="O20" s="125"/>
+      <c r="P20" s="120"/>
     </row>
     <row r="21" spans="1:16" ht="13.95" customHeight="1">
-      <c r="M21" s="108"/>
-      <c r="N21" s="111"/>
-      <c r="O21" s="111"/>
-      <c r="P21" s="114"/>
+      <c r="M21" s="129"/>
+      <c r="N21" s="131"/>
+      <c r="O21" s="131"/>
+      <c r="P21" s="121"/>
     </row>
     <row r="22" spans="1:16" ht="13.95" customHeight="1">
-      <c r="M22" s="109"/>
-      <c r="N22" s="112"/>
-      <c r="O22" s="112"/>
-      <c r="P22" s="115"/>
+      <c r="M22" s="124"/>
+      <c r="N22" s="126"/>
+      <c r="O22" s="126"/>
+      <c r="P22" s="134"/>
     </row>
     <row r="23" spans="1:16" ht="15.6">
-      <c r="A23" s="96" t="s">
+      <c r="A23" s="100" t="s">
         <v>602</v>
       </c>
-      <c r="B23" s="96"/>
-      <c r="C23" s="96"/>
-      <c r="D23" s="96"/>
-      <c r="E23" s="96"/>
+      <c r="B23" s="100"/>
+      <c r="C23" s="100"/>
+      <c r="D23" s="100"/>
+      <c r="E23" s="100"/>
       <c r="F23" s="81"/>
       <c r="M23" s="60" t="s">
         <v>89</v>
@@ -9496,13 +9523,13 @@
         <v>414</v>
       </c>
       <c r="F25" s="41"/>
-      <c r="M25" s="107" t="s">
+      <c r="M25" s="123" t="s">
         <v>92</v>
       </c>
-      <c r="N25" s="110" t="s">
+      <c r="N25" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="O25" s="117"/>
+      <c r="O25" s="127"/>
       <c r="P25" s="62"/>
     </row>
     <row r="26" spans="1:16" ht="13.95" customHeight="1">
@@ -9522,9 +9549,9 @@
         <v>590</v>
       </c>
       <c r="F26" s="80"/>
-      <c r="M26" s="109"/>
-      <c r="N26" s="112"/>
-      <c r="O26" s="118"/>
+      <c r="M26" s="124"/>
+      <c r="N26" s="126"/>
+      <c r="O26" s="128"/>
       <c r="P26" s="64"/>
     </row>
     <row r="27" spans="1:16" ht="13.95" customHeight="1">
@@ -9544,14 +9571,14 @@
         <v>589</v>
       </c>
       <c r="F27" s="80"/>
-      <c r="M27" s="107" t="s">
+      <c r="M27" s="123" t="s">
         <v>93</v>
       </c>
-      <c r="N27" s="110" t="s">
+      <c r="N27" s="125" t="s">
         <v>91</v>
       </c>
-      <c r="O27" s="110"/>
-      <c r="P27" s="113"/>
+      <c r="O27" s="125"/>
+      <c r="P27" s="120"/>
     </row>
     <row r="28" spans="1:16" ht="13.95" customHeight="1">
       <c r="A28" s="41" t="s">
@@ -9570,10 +9597,10 @@
         <v>591</v>
       </c>
       <c r="F28" s="80"/>
-      <c r="M28" s="108"/>
-      <c r="N28" s="111"/>
-      <c r="O28" s="111"/>
-      <c r="P28" s="114"/>
+      <c r="M28" s="129"/>
+      <c r="N28" s="131"/>
+      <c r="O28" s="131"/>
+      <c r="P28" s="121"/>
     </row>
     <row r="29" spans="1:16" ht="13.95" customHeight="1">
       <c r="A29" s="41" t="s">
@@ -9592,10 +9619,10 @@
         <v>592</v>
       </c>
       <c r="F29" s="80"/>
-      <c r="M29" s="108"/>
-      <c r="N29" s="111"/>
-      <c r="O29" s="111"/>
-      <c r="P29" s="114"/>
+      <c r="M29" s="129"/>
+      <c r="N29" s="131"/>
+      <c r="O29" s="131"/>
+      <c r="P29" s="121"/>
     </row>
     <row r="30" spans="1:16" ht="14.4" customHeight="1" thickBot="1">
       <c r="A30" s="41" t="s">
@@ -9614,10 +9641,10 @@
         <v>593</v>
       </c>
       <c r="F30" s="80"/>
-      <c r="M30" s="119"/>
-      <c r="N30" s="120"/>
-      <c r="O30" s="120"/>
-      <c r="P30" s="116"/>
+      <c r="M30" s="130"/>
+      <c r="N30" s="132"/>
+      <c r="O30" s="132"/>
+      <c r="P30" s="122"/>
     </row>
     <row r="31" spans="1:16">
       <c r="A31" s="41" t="s">
@@ -9851,6 +9878,23 @@
     </row>
   </sheetData>
   <mergeCells count="33">
+    <mergeCell ref="A23:E23"/>
+    <mergeCell ref="O12:O15"/>
+    <mergeCell ref="M5:M7"/>
+    <mergeCell ref="N5:N7"/>
+    <mergeCell ref="O5:O7"/>
+    <mergeCell ref="P5:P7"/>
+    <mergeCell ref="M20:M22"/>
+    <mergeCell ref="N20:N22"/>
+    <mergeCell ref="O20:O22"/>
+    <mergeCell ref="P20:P22"/>
+    <mergeCell ref="P27:P30"/>
+    <mergeCell ref="M25:M26"/>
+    <mergeCell ref="N25:N26"/>
+    <mergeCell ref="O25:O26"/>
+    <mergeCell ref="M27:M30"/>
+    <mergeCell ref="N27:N30"/>
+    <mergeCell ref="O27:O30"/>
     <mergeCell ref="B1:C1"/>
     <mergeCell ref="B7:C7"/>
     <mergeCell ref="M1:P1"/>
@@ -9867,23 +9911,6 @@
     <mergeCell ref="O10:O11"/>
     <mergeCell ref="M12:M15"/>
     <mergeCell ref="N12:N15"/>
-    <mergeCell ref="P27:P30"/>
-    <mergeCell ref="M25:M26"/>
-    <mergeCell ref="N25:N26"/>
-    <mergeCell ref="O25:O26"/>
-    <mergeCell ref="M27:M30"/>
-    <mergeCell ref="N27:N30"/>
-    <mergeCell ref="O27:O30"/>
-    <mergeCell ref="P5:P7"/>
-    <mergeCell ref="M20:M22"/>
-    <mergeCell ref="N20:N22"/>
-    <mergeCell ref="O20:O22"/>
-    <mergeCell ref="P20:P22"/>
-    <mergeCell ref="A23:E23"/>
-    <mergeCell ref="O12:O15"/>
-    <mergeCell ref="M5:M7"/>
-    <mergeCell ref="N5:N7"/>
-    <mergeCell ref="O5:O7"/>
   </mergeCells>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
@@ -10155,7 +10182,7 @@
   <dimension ref="A1:K36"/>
   <sheetViews>
     <sheetView workbookViewId="0">
-      <selection sqref="A1:B1"/>
+      <selection activeCell="B12" sqref="B12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.8"/>
@@ -10172,29 +10199,29 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:11">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="100" t="s">
         <v>117</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="D1" s="96" t="s">
+      <c r="B1" s="100"/>
+      <c r="D1" s="100" t="s">
         <v>587</v>
       </c>
-      <c r="E1" s="96"/>
-      <c r="G1" s="96" t="s">
+      <c r="E1" s="100"/>
+      <c r="G1" s="100" t="s">
         <v>122</v>
       </c>
-      <c r="H1" s="96"/>
-      <c r="J1" s="96" t="s">
+      <c r="H1" s="100"/>
+      <c r="J1" s="100" t="s">
         <v>588</v>
       </c>
-      <c r="K1" s="96"/>
+      <c r="K1" s="100"/>
     </row>
     <row r="2" spans="1:11" ht="15.6">
       <c r="A2" s="40" t="s">
-        <v>28</v>
+        <v>656</v>
       </c>
       <c r="B2" s="40" t="s">
-        <v>605</v>
+        <v>657</v>
       </c>
       <c r="D2" s="40" t="s">
         <v>638</v>
@@ -10323,7 +10350,12 @@
       <c r="H9" s="65"/>
     </row>
     <row r="10" spans="1:11" ht="14.4">
-      <c r="A10" s="78"/>
+      <c r="A10" s="65" t="s">
+        <v>119</v>
+      </c>
+      <c r="B10" s="78">
+        <v>450640112</v>
+      </c>
       <c r="D10" s="65"/>
       <c r="E10" s="65"/>
       <c r="F10" s="65"/>
@@ -10612,17 +10644,17 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:14" ht="19.2" customHeight="1">
-      <c r="A1" s="96" t="s">
+      <c r="A1" s="100" t="s">
         <v>654</v>
       </c>
-      <c r="B1" s="96"/>
-      <c r="C1" s="96"/>
-      <c r="D1" s="96"/>
-      <c r="E1" s="96"/>
-      <c r="F1" s="96"/>
-      <c r="G1" s="96"/>
-      <c r="H1" s="96"/>
-      <c r="I1" s="96"/>
+      <c r="B1" s="100"/>
+      <c r="C1" s="100"/>
+      <c r="D1" s="100"/>
+      <c r="E1" s="100"/>
+      <c r="F1" s="100"/>
+      <c r="G1" s="100"/>
+      <c r="H1" s="100"/>
+      <c r="I1" s="100"/>
       <c r="N1" s="40"/>
     </row>
     <row r="2" spans="1:14" ht="15.6">
@@ -10658,7 +10690,7 @@
       <c r="A3" t="s">
         <v>137</v>
       </c>
-      <c r="B3" s="138" t="s">
+      <c r="B3" s="86" t="s">
         <v>649</v>
       </c>
       <c r="D3" t="s">
@@ -10678,7 +10710,7 @@
       <c r="A4" t="s">
         <v>137</v>
       </c>
-      <c r="B4" s="138" t="s">
+      <c r="B4" s="86" t="s">
         <v>650</v>
       </c>
       <c r="D4" t="s">
@@ -10724,10 +10756,10 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A1" s="134" t="s">
+      <c r="A1" s="135" t="s">
         <v>140</v>
       </c>
-      <c r="B1" s="135"/>
+      <c r="B1" s="136"/>
     </row>
     <row r="2" spans="1:2" ht="15.6">
       <c r="A2" s="55" t="s">
@@ -10856,10 +10888,10 @@
       <c r="B21" s="14"/>
     </row>
     <row r="22" spans="1:2" ht="15.6" customHeight="1">
-      <c r="A22" s="136" t="s">
+      <c r="A22" s="137" t="s">
         <v>140</v>
       </c>
-      <c r="B22" s="137"/>
+      <c r="B22" s="138"/>
     </row>
     <row r="23" spans="1:2" ht="15.6">
       <c r="A23" s="57" t="s">

</xml_diff>